<commit_message>
Project signup time over! Update final signup list
</commit_message>
<xml_diff>
--- a/Courses/ProjectSignUp.xlsx
+++ b/Courses/ProjectSignUp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\我的坚果云\My_Work\1989chenguo.github.io\Courses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/MyNutStore/My_Work/1989chenguo.github.io/Courses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2559352D-3E64-410A-BA5E-74451BEA7993}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8B3CAF-74EB-A64F-A8EB-12D256E53367}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11745" windowHeight="7095" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="报名表" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="166">
   <si>
     <t>姓名 </t>
   </si>
@@ -518,6 +518,13 @@
   </si>
   <si>
     <t>否</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>组长</t>
+    <rPh sb="0" eb="2">
+      <t>zu zhang</t>
+    </rPh>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -534,19 +541,23 @@
     <font>
       <sz val="9"/>
       <name val="PingFang SC"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="PingFang SC"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="PingFang SC"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="30"/>
       <color rgb="FFFE2C23"/>
       <name val="PingFang SC"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -947,14 +958,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041410A3-A696-47D7-A0D7-3E745762DC13}">
   <dimension ref="A1:G196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="G155" sqref="G155"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="J172" sqref="J172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="16.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.19921875" defaultRowHeight="16.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" customWidth="1"/>
+    <col min="2" max="7" width="9.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1">
@@ -3288,9 +3299,15 @@
       <c r="A152" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B152" s="7"/>
-      <c r="C152" s="6"/>
-      <c r="D152" s="7"/>
+      <c r="B152" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C152" s="6">
+        <v>32</v>
+      </c>
+      <c r="D152" s="7" t="s">
+        <v>165</v>
+      </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>

</xml_diff>